<commit_message>
twee trammetjes rijden na elkaar met eindhaltes
</commit_message>
<xml_diff>
--- a/input_analysis/_data/afstanden&rijtijden.xlsx
+++ b/input_analysis/_data/afstanden&rijtijden.xlsx
@@ -11,12 +11,41 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Blad1!$O$6</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Blad1!$N$6</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>Stop</t>
   </si>
@@ -73,6 +102,27 @@
   </si>
   <si>
     <t>km/uur^2</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>min</t>
   </si>
 </sst>
 </file>
@@ -455,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,9 +516,11 @@
     <col min="1" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -497,8 +549,29 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -519,8 +592,47 @@
         <f>C3/(D3/3600)^2</f>
         <v>1010.4700378703499</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <f>0.0002*F3^2-0.843*F3+1020.7</f>
+        <v>373.08369756203638</v>
+      </c>
+      <c r="I3">
+        <f>D3/60</f>
+        <v>2.2333333333333334</v>
+      </c>
+      <c r="J3">
+        <f>G3/60</f>
+        <v>6.2180616260339399</v>
+      </c>
+      <c r="L3">
+        <v>1.48999530146229</v>
+      </c>
+      <c r="M3">
+        <f>SQRT(LN(J3/I3^2+1))</f>
+        <v>0.89969135947549284</v>
+      </c>
+      <c r="O3">
+        <f>LN(I3)-LN(SQRT(J3/I3^2+1))</f>
+        <v>0.39877296657138039</v>
+      </c>
+      <c r="P3">
+        <f>EXP(O3)</f>
+        <v>1.4899953014622869</v>
+      </c>
+      <c r="Q3">
+        <f>SQRT(LN(1+J3/I3^2))</f>
+        <v>0.89969135947549284</v>
+      </c>
+      <c r="R3">
+        <f>(EXP(Q3^2)-1)*EXP(2*O3+Q3^2)</f>
+        <v>6.2180616260339416</v>
+      </c>
+      <c r="T3">
+        <f>(C3-0.097)/70*60+1/6</f>
+        <v>1.2835238095238095</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -538,11 +650,46 @@
         <v>45.925925925925924</v>
       </c>
       <c r="F4" s="4">
-        <f t="shared" ref="F4:F21" si="1">C4/(D4/3600)^2</f>
+        <f>C4/(D4/3600)^2</f>
         <v>680.38408779149518</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <f t="shared" ref="G4:G21" si="1">0.0002*F4^2-0.843*F4+1020.7</f>
+        <v>539.72071537574266</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I21" si="2">D4/60</f>
+        <v>4.05</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J21" si="3">G4/60</f>
+        <v>8.995345256262377</v>
+      </c>
+      <c r="L4">
+        <v>3.2547048421015639</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M21" si="4">SQRT(LN(J4/I4^2+1))</f>
+        <v>0.66123413081790183</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O21" si="5">LN(I4)-LN(SQRT(J4/I4^2+1))</f>
+        <v>1.1801015932391947</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P21" si="6">EXP(O4)</f>
+        <v>3.2547048421015639</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q21" si="7">SQRT(LN(1+J4/I4^2))</f>
+        <v>0.66123413081790183</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T21" si="8">(C4-0.097)/70*60+1/6</f>
+        <v>2.7406666666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -560,11 +707,46 @@
         <v>36.610169491525419</v>
       </c>
       <c r="F5" s="4">
+        <f t="shared" ref="F5:F21" si="9">C5/(D5/3600)^2</f>
+        <v>2233.840850330364</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="1"/>
-        <v>2233.840850330364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>135.58115209243999</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0.98333333333333328</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>2.2596858682073333</v>
+      </c>
+      <c r="L5">
+        <v>0.53830314576661209</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>1.0977488703931864</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
+        <v>-0.61933340954113958</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="6"/>
+        <v>0.5383031457666122</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="7"/>
+        <v>1.0977488703931864</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="8"/>
+        <v>0.59780952380952379</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -582,11 +764,46 @@
         <v>28.514851485148515</v>
       </c>
       <c r="F6" s="4">
+        <f t="shared" si="9"/>
+        <v>1016.3709440250957</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="1"/>
-        <v>1016.3709440250957</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>370.50127335853722</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>1.6833333333333333</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>6.1750212226422869</v>
+      </c>
+      <c r="L6">
+        <v>0.94408438713276877</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>1.0754679709800801</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>-5.7539723682846322E-2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
+        <v>0.94408438713276877</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="7"/>
+        <v>1.0754679709800801</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="8"/>
+        <v>0.76923809523809528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -604,11 +821,46 @@
         <v>24</v>
       </c>
       <c r="F7" s="4">
+        <f t="shared" si="9"/>
+        <v>1440</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="1"/>
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>221.5</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>3.6916666666666669</v>
+      </c>
+      <c r="L7">
+        <v>0.46167507200809177</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>1.2432971830409834</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>-0.77289394267882228</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>0.46167507200809177</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="7"/>
+        <v>1.2432971830409834</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="8"/>
+        <v>0.42638095238095242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -626,11 +878,46 @@
         <v>16.744186046511629</v>
       </c>
       <c r="F8" s="4">
+        <f t="shared" si="9"/>
+        <v>700.91941590048668</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="1"/>
-        <v>700.91941590048668</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>528.08253791314576</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>1.4333333333333333</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>8.8013756318857634</v>
+      </c>
+      <c r="L8">
+        <v>0.62353822643420043</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>1.2902309408283692</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>-0.47234520630402244</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>0.62353822643420032</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="7"/>
+        <v>1.2902309408283692</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="8"/>
+        <v>0.42638095238095242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -641,16 +928,25 @@
       <c r="D9" s="2">
         <v>78</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>27.69230769230769</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="1"/>
-        <v>1278.1065088757396</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F9" s="4"/>
+      <c r="O9" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P9" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q9" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="8"/>
+        <v>0.59780952380952379</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -661,19 +957,44 @@
       <c r="D10" s="2">
         <v>113</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>19.115044247787608</v>
-      </c>
-      <c r="F10" s="4">
-        <f t="shared" si="1"/>
-        <v>608.97486099146374</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="4"/>
+      <c r="O10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P10" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q10" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="8"/>
+        <v>0.59780952380952379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O11" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P11" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q11" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="8"/>
+        <v>8.3523809523809514E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,8 +1008,24 @@
         <v>3</v>
       </c>
       <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="O12" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P12" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q12" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T12" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -696,8 +1033,24 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="O13" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P13" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q13" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="8"/>
+        <v>8.3523809523809514E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -708,16 +1061,25 @@
       <c r="D14" s="2">
         <v>110</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>19.636363636363637</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="1"/>
-        <v>642.64462809917359</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="4"/>
+      <c r="O14" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P14" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q14" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="8"/>
+        <v>0.59780952380952379</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -730,16 +1092,25 @@
       <c r="D15" s="2">
         <v>78</v>
       </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>27.69230769230769</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="1"/>
-        <v>1278.1065088757396</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F15" s="4"/>
+      <c r="O15" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P15" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q15" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="8"/>
+        <v>0.59780952380952379</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -757,11 +1128,46 @@
         <v>17.560975609756099</v>
       </c>
       <c r="F16" s="4">
+        <f t="shared" si="9"/>
+        <v>770.96966091612126</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="1"/>
-        <v>770.96966091612126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>489.65141945833363</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>1.3666666666666667</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>8.1608569909722277</v>
+      </c>
+      <c r="L16">
+        <v>0.58979935931293559</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>1.2964162556233334</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="5"/>
+        <v>-0.52797286888005979</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="6"/>
+        <v>0.58979935931293559</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="7"/>
+        <v>1.2964162556233334</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="8"/>
+        <v>0.42638095238095242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -779,11 +1185,46 @@
         <v>24</v>
       </c>
       <c r="F17" s="4">
+        <f t="shared" si="9"/>
+        <v>1440</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="1"/>
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>221.5</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>3.6916666666666669</v>
+      </c>
+      <c r="L17">
+        <v>0.46167507200809177</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>1.2432971830409834</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="5"/>
+        <v>-0.77289394267882228</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="6"/>
+        <v>0.46167507200809177</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="7"/>
+        <v>1.2432971830409834</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="8"/>
+        <v>0.42638095238095242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -801,11 +1242,46 @@
         <v>28.800000000000004</v>
       </c>
       <c r="F18" s="4">
+        <f t="shared" si="9"/>
+        <v>1036.8000000000002</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="1"/>
-        <v>1036.8000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>361.66844800000001</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>6.0278074666666672</v>
+      </c>
+      <c r="L18">
+        <v>0.93609168243672192</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="4"/>
+        <v>1.0741205516571863</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="5"/>
+        <v>-6.604185598017831E-2</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="6"/>
+        <v>0.93609168243672192</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="7"/>
+        <v>1.0741205516571863</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="8"/>
+        <v>0.76923809523809528</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -823,11 +1299,46 @@
         <v>36.610169491525419</v>
       </c>
       <c r="F19" s="4">
+        <f t="shared" si="9"/>
+        <v>2233.840850330364</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="1"/>
-        <v>2233.840850330364</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>135.58115209243999</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>0.98333333333333328</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>2.2596858682073333</v>
+      </c>
+      <c r="L19">
+        <v>0.53830314576661209</v>
+      </c>
+      <c r="M19">
+        <f>SQRT(LN(J19/I19^2+1))</f>
+        <v>1.0977488703931864</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="5"/>
+        <v>-0.61933340954113958</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="6"/>
+        <v>0.5383031457666122</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="7"/>
+        <v>1.0977488703931864</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="8"/>
+        <v>0.59780952380952379</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
@@ -845,11 +1356,46 @@
         <v>45.925925925925924</v>
       </c>
       <c r="F20" s="4">
+        <f t="shared" si="9"/>
+        <v>680.38408779149518</v>
+      </c>
+      <c r="G20">
         <f t="shared" si="1"/>
-        <v>680.38408779149518</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>539.72071537574266</v>
+      </c>
+      <c r="I20">
+        <f>D20/60</f>
+        <v>4.05</v>
+      </c>
+      <c r="J20">
+        <f>G20/60</f>
+        <v>8.995345256262377</v>
+      </c>
+      <c r="L20">
+        <v>3.2547048421015639</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="4"/>
+        <v>0.66123413081790183</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="5"/>
+        <v>1.1801015932391947</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="6"/>
+        <v>3.2547048421015639</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="7"/>
+        <v>0.66123413081790183</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="8"/>
+        <v>2.7406666666666664</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -867,8 +1413,43 @@
         <v>37.333333333333336</v>
       </c>
       <c r="F21" s="4">
+        <f t="shared" si="9"/>
+        <v>995.55555555555554</v>
+      </c>
+      <c r="G21">
         <f t="shared" si="1"/>
-        <v>995.55555555555554</v>
+        <v>379.67283950617286</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>6.3278806584362144</v>
+      </c>
+      <c r="L21">
+        <v>1.5000160885922571</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="4"/>
+        <v>0.90050472784712587</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="5"/>
+        <v>0.40547583377881563</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="6"/>
+        <v>1.5000160885922571</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="7"/>
+        <v>0.90050472784712587</v>
+      </c>
+      <c r="T21">
+        <f>(C21-0.097)/70*60+1/6</f>
+        <v>1.2835238095238095</v>
       </c>
     </row>
   </sheetData>

</xml_diff>